<commit_message>
Funciona funcao de troca de display a quente, porem o salvar de status parou de funcionar
</commit_message>
<xml_diff>
--- a/Mapa de Memoria/Mapa de memoria interna da placa Mae.xlsx
+++ b/Mapa de Memoria/Mapa de memoria interna da placa Mae.xlsx
@@ -159,6 +159,20 @@
             <charset val="1"/>
           </rPr>
           <t xml:space="preserve">Tempo de captura do DataLog</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="L17" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">Resolucao do Display</t>
         </r>
       </text>
     </comment>
@@ -587,14 +601,14 @@
   <dimension ref="A1:Q65"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B8" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="A8" activeCellId="0" sqref="A8"/>
-      <selection pane="bottomRight" activeCell="L16" activeCellId="0" sqref="L16"/>
+      <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="L17" activeCellId="0" sqref="L17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6953125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.70703125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="4.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="2" style="0" width="3.71"/>
@@ -980,8 +994,8 @@
       <c r="I17" s="12"/>
       <c r="J17" s="12"/>
       <c r="K17" s="13"/>
-      <c r="L17" s="1"/>
-      <c r="M17" s="1"/>
+      <c r="L17" s="6"/>
+      <c r="M17" s="6"/>
       <c r="N17" s="1"/>
       <c r="O17" s="1"/>
       <c r="P17" s="2"/>
@@ -2018,7 +2032,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6953125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.70703125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.511805555555555" right="0.511805555555555" top="0.7875" bottom="0.7875" header="0.511805555555555" footer="0.511805555555555"/>
@@ -2041,7 +2055,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6953125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.70703125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.511805555555555" right="0.511805555555555" top="0.7875" bottom="0.7875" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>

<commit_message>
Sera implementado funcao de exibiçao de grafico em uma unica tela
</commit_message>
<xml_diff>
--- a/Mapa de Memoria/Mapa de memoria interna da placa Mae.xlsx
+++ b/Mapa de Memoria/Mapa de memoria interna da placa Mae.xlsx
@@ -605,10 +605,10 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="L17" activeCellId="0" sqref="L17"/>
+      <selection pane="bottomRight" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.70703125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.72265625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="4.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="2" style="0" width="3.71"/>
@@ -665,7 +665,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="n">
         <v>0</v>
       </c>
@@ -2032,7 +2032,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.70703125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.72265625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.511805555555555" right="0.511805555555555" top="0.7875" bottom="0.7875" header="0.511805555555555" footer="0.511805555555555"/>
@@ -2055,7 +2055,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.70703125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.72265625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.511805555555555" right="0.511805555555555" top="0.7875" bottom="0.7875" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>